<commit_message>
Correcting 4 rep experiment metadata
</commit_message>
<xml_diff>
--- a/info/Design_experiments_4rep.xlsx
+++ b/info/Design_experiments_4rep.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MGierlinski/Work/Projects/NCCProt/info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E777EE-22A6-D840-9335-300DB2E5A0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F173270-3FB4-EC4E-B522-F7B242CF78C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8420" yWindow="1160" windowWidth="29040" windowHeight="25300" xr2:uid="{E3A6127A-0016-0143-8635-61EDB91F9D25}"/>
+    <workbookView xWindow="8420" yWindow="500" windowWidth="29040" windowHeight="21100" xr2:uid="{E3A6127A-0016-0143-8635-61EDB91F9D25}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment 1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="127">
   <si>
     <t>Sample name</t>
   </si>
@@ -357,9 +357,6 @@
     <t>TMT-batch</t>
   </si>
   <si>
-    <t>Channel 2 (127N) and 9 (130C) are empty channels. Chanel 10 (131) is the reference channel within 3 batches (ignore this usually don't need).</t>
-  </si>
-  <si>
     <t>Nas_DMSO_IP_4</t>
   </si>
   <si>
@@ -378,26 +375,65 @@
     <t>2h_DRB_IP_4</t>
   </si>
   <si>
-    <t>Nas_TPL_Input_4</t>
-  </si>
-  <si>
-    <t>1h_TPL_Input_4</t>
-  </si>
-  <si>
-    <t>2h_TPL_Input_4</t>
-  </si>
-  <si>
     <t>NegCtl_IP_4</t>
+  </si>
+  <si>
+    <t>Nas_TPL_IP_4</t>
+  </si>
+  <si>
+    <t>1h_TPL_IP_4</t>
+  </si>
+  <si>
+    <t>2h_TPL_IP_4</t>
+  </si>
+  <si>
+    <t>SB72</t>
+  </si>
+  <si>
+    <t>SB73</t>
+  </si>
+  <si>
+    <t>SB74</t>
+  </si>
+  <si>
+    <t>batch</t>
+  </si>
+  <si>
+    <t>SB45-IP</t>
+  </si>
+  <si>
+    <t>SB45-LI</t>
+  </si>
+  <si>
+    <t>SB46-IP</t>
+  </si>
+  <si>
+    <t>SB46-LI</t>
+  </si>
+  <si>
+    <t>SB47-IP</t>
+  </si>
+  <si>
+    <t>SB47-LI</t>
+  </si>
+  <si>
+    <t>SB81-IP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -423,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -431,6 +467,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -746,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05AE7BCD-536C-EC44-BBCE-0E3BE6E6495C}">
-  <dimension ref="A1:L71"/>
+  <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="L72" sqref="L72"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="P60" sqref="P60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -763,7 +805,7 @@
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -800,8 +842,11 @@
       <c r="L1" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -835,11 +880,14 @@
       <c r="K2" s="2">
         <v>1</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="5">
         <v>126</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -873,11 +921,14 @@
       <c r="K3" s="2">
         <v>2</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -911,11 +962,14 @@
       <c r="K4" s="2">
         <v>3</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -949,11 +1003,14 @@
       <c r="K5" s="2">
         <v>4</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -987,11 +1044,14 @@
       <c r="K6" s="2">
         <v>5</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1025,11 +1085,14 @@
       <c r="K7" s="2">
         <v>6</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1063,11 +1126,14 @@
       <c r="K8" s="2">
         <v>7</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1101,11 +1167,14 @@
       <c r="K9" s="2">
         <v>8</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1139,11 +1208,14 @@
       <c r="K10" s="2">
         <v>9</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1177,11 +1249,14 @@
       <c r="K11" s="2">
         <v>10</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="5">
         <v>131</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1215,11 +1290,14 @@
       <c r="K12" s="2">
         <v>1</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="5">
         <v>126</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1253,11 +1331,14 @@
       <c r="K13" s="2">
         <v>2</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1291,11 +1372,14 @@
       <c r="K14" s="2">
         <v>3</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1329,11 +1413,14 @@
       <c r="K15" s="2">
         <v>4</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="L15" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1367,11 +1454,14 @@
       <c r="K16" s="2">
         <v>5</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="L16" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1405,11 +1495,14 @@
       <c r="K17" s="2">
         <v>6</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L17" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1443,11 +1536,14 @@
       <c r="K18" s="2">
         <v>7</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="L18" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -1481,11 +1577,14 @@
       <c r="K19" s="2">
         <v>8</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="L19" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -1519,11 +1618,14 @@
       <c r="K20" s="2">
         <v>9</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="L20" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1557,11 +1659,14 @@
       <c r="K21" s="2">
         <v>10</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L21" s="5">
         <v>131</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1595,11 +1700,14 @@
       <c r="K22" s="2">
         <v>1</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L22" s="5">
         <v>126</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1633,11 +1741,14 @@
       <c r="K23" s="2">
         <v>2</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="L23" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1671,11 +1782,14 @@
       <c r="K24" s="2">
         <v>3</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="L24" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1709,11 +1823,14 @@
       <c r="K25" s="2">
         <v>4</v>
       </c>
-      <c r="L25" s="2" t="s">
+      <c r="L25" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1747,11 +1864,14 @@
       <c r="K26" s="2">
         <v>5</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="L26" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1785,11 +1905,14 @@
       <c r="K27" s="2">
         <v>6</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="L27" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1823,11 +1946,14 @@
       <c r="K28" s="2">
         <v>7</v>
       </c>
-      <c r="L28" s="2" t="s">
+      <c r="L28" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1861,11 +1987,14 @@
       <c r="K29" s="2">
         <v>8</v>
       </c>
-      <c r="L29" s="2" t="s">
+      <c r="L29" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1899,11 +2028,14 @@
       <c r="K30" s="2">
         <v>9</v>
       </c>
-      <c r="L30" s="2" t="s">
+      <c r="L30" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1937,11 +2069,14 @@
       <c r="K31" s="2">
         <v>10</v>
       </c>
-      <c r="L31" s="2">
+      <c r="L31" s="5">
         <v>131</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1975,11 +2110,14 @@
       <c r="K32" s="2">
         <v>1</v>
       </c>
-      <c r="L32" s="2">
+      <c r="L32" s="5">
         <v>126</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -2013,11 +2151,14 @@
       <c r="K33" s="2">
         <v>2</v>
       </c>
-      <c r="L33" s="2" t="s">
+      <c r="L33" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -2051,11 +2192,14 @@
       <c r="K34" s="2">
         <v>3</v>
       </c>
-      <c r="L34" s="2" t="s">
+      <c r="L34" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -2089,11 +2233,14 @@
       <c r="K35" s="2">
         <v>4</v>
       </c>
-      <c r="L35" s="2" t="s">
+      <c r="L35" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -2127,11 +2274,14 @@
       <c r="K36" s="2">
         <v>5</v>
       </c>
-      <c r="L36" s="2" t="s">
+      <c r="L36" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -2165,11 +2315,14 @@
       <c r="K37" s="2">
         <v>6</v>
       </c>
-      <c r="L37" s="2" t="s">
+      <c r="L37" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -2203,11 +2356,14 @@
       <c r="K38" s="2">
         <v>7</v>
       </c>
-      <c r="L38" s="2" t="s">
+      <c r="L38" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M38" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -2241,11 +2397,14 @@
       <c r="K39" s="2">
         <v>8</v>
       </c>
-      <c r="L39" s="2" t="s">
+      <c r="L39" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -2279,11 +2438,14 @@
       <c r="K40" s="2">
         <v>9</v>
       </c>
-      <c r="L40" s="2" t="s">
+      <c r="L40" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M40" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>57</v>
       </c>
@@ -2317,11 +2479,14 @@
       <c r="K41" s="2">
         <v>10</v>
       </c>
-      <c r="L41" s="2">
+      <c r="L41" s="5">
         <v>131</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M41" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2355,11 +2520,14 @@
       <c r="K42" s="2">
         <v>1</v>
       </c>
-      <c r="L42" s="2">
+      <c r="L42" s="5">
         <v>126</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M42" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>59</v>
       </c>
@@ -2393,11 +2561,14 @@
       <c r="K43" s="2">
         <v>2</v>
       </c>
-      <c r="L43" s="2" t="s">
+      <c r="L43" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>60</v>
       </c>
@@ -2431,11 +2602,14 @@
       <c r="K44" s="2">
         <v>3</v>
       </c>
-      <c r="L44" s="2" t="s">
+      <c r="L44" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M44" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>61</v>
       </c>
@@ -2469,11 +2643,14 @@
       <c r="K45" s="2">
         <v>4</v>
       </c>
-      <c r="L45" s="2" t="s">
+      <c r="L45" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>62</v>
       </c>
@@ -2507,11 +2684,14 @@
       <c r="K46" s="2">
         <v>5</v>
       </c>
-      <c r="L46" s="2" t="s">
+      <c r="L46" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>63</v>
       </c>
@@ -2545,11 +2725,14 @@
       <c r="K47" s="2">
         <v>6</v>
       </c>
-      <c r="L47" s="2" t="s">
+      <c r="L47" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M47" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>64</v>
       </c>
@@ -2583,11 +2766,14 @@
       <c r="K48" s="2">
         <v>7</v>
       </c>
-      <c r="L48" s="2" t="s">
+      <c r="L48" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M48" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>65</v>
       </c>
@@ -2621,11 +2807,14 @@
       <c r="K49" s="2">
         <v>8</v>
       </c>
-      <c r="L49" s="2" t="s">
+      <c r="L49" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M49" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>66</v>
       </c>
@@ -2659,11 +2848,14 @@
       <c r="K50" s="2">
         <v>9</v>
       </c>
-      <c r="L50" s="2" t="s">
+      <c r="L50" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M50" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>67</v>
       </c>
@@ -2697,11 +2889,14 @@
       <c r="K51" s="2">
         <v>10</v>
       </c>
-      <c r="L51" s="2">
+      <c r="L51" s="5">
         <v>131</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>68</v>
       </c>
@@ -2735,11 +2930,14 @@
       <c r="K52" s="2">
         <v>1</v>
       </c>
-      <c r="L52" s="2">
+      <c r="L52" s="5">
         <v>126</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M52" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>69</v>
       </c>
@@ -2773,11 +2971,14 @@
       <c r="K53" s="2">
         <v>2</v>
       </c>
-      <c r="L53" s="2" t="s">
+      <c r="L53" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M53" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>70</v>
       </c>
@@ -2811,11 +3012,14 @@
       <c r="K54" s="2">
         <v>3</v>
       </c>
-      <c r="L54" s="2" t="s">
+      <c r="L54" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>71</v>
       </c>
@@ -2849,11 +3053,14 @@
       <c r="K55" s="2">
         <v>4</v>
       </c>
-      <c r="L55" s="2" t="s">
+      <c r="L55" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M55" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>72</v>
       </c>
@@ -2887,11 +3094,14 @@
       <c r="K56" s="2">
         <v>5</v>
       </c>
-      <c r="L56" s="2" t="s">
+      <c r="L56" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M56" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>73</v>
       </c>
@@ -2925,11 +3135,14 @@
       <c r="K57" s="2">
         <v>6</v>
       </c>
-      <c r="L57" s="2" t="s">
+      <c r="L57" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M57" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>74</v>
       </c>
@@ -2963,11 +3176,14 @@
       <c r="K58" s="2">
         <v>7</v>
       </c>
-      <c r="L58" s="2" t="s">
+      <c r="L58" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M58" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>75</v>
       </c>
@@ -3001,11 +3217,14 @@
       <c r="K59" s="2">
         <v>8</v>
       </c>
-      <c r="L59" s="2" t="s">
+      <c r="L59" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M59" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>76</v>
       </c>
@@ -3039,11 +3258,14 @@
       <c r="K60" s="2">
         <v>9</v>
       </c>
-      <c r="L60" s="2" t="s">
+      <c r="L60" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M60" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>77</v>
       </c>
@@ -3077,13 +3299,16 @@
       <c r="K61" s="2">
         <v>10</v>
       </c>
-      <c r="L61" s="2">
+      <c r="L61" s="5">
         <v>131</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M61" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s">
         <v>7</v>
@@ -3115,13 +3340,16 @@
       <c r="K62" s="2">
         <v>10</v>
       </c>
-      <c r="L62" s="2">
+      <c r="L62" s="5">
         <v>131</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B63" t="s">
         <v>6</v>
@@ -3153,13 +3381,16 @@
       <c r="K63" s="2">
         <v>9</v>
       </c>
-      <c r="L63" s="2" t="s">
+      <c r="L63" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M63" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B64" t="s">
         <v>7</v>
@@ -3191,13 +3422,16 @@
       <c r="K64" s="2">
         <v>8</v>
       </c>
-      <c r="L64" s="2" t="s">
+      <c r="L64" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M64" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B65" t="s">
         <v>7</v>
@@ -3229,13 +3463,16 @@
       <c r="K65" s="2">
         <v>7</v>
       </c>
-      <c r="L65" s="2" t="s">
+      <c r="L65" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M65" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B66" t="s">
         <v>6</v>
@@ -3250,10 +3487,10 @@
         <v>7</v>
       </c>
       <c r="F66" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G66" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H66" t="s">
         <v>16</v>
@@ -3267,13 +3504,16 @@
       <c r="K66" s="2">
         <v>6</v>
       </c>
-      <c r="L66" s="2" t="s">
+      <c r="L66" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M66" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B67" t="s">
         <v>7</v>
@@ -3288,10 +3528,10 @@
         <v>7</v>
       </c>
       <c r="F67" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H67" t="s">
         <v>16</v>
@@ -3305,13 +3545,16 @@
       <c r="K67" s="2">
         <v>5</v>
       </c>
-      <c r="L67" s="2" t="s">
+      <c r="L67" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M67" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B68" t="s">
         <v>7</v>
@@ -3326,10 +3569,10 @@
         <v>7</v>
       </c>
       <c r="F68" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G68" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H68" t="s">
         <v>16</v>
@@ -3343,11 +3586,14 @@
       <c r="K68" s="2">
         <v>4</v>
       </c>
-      <c r="L68" s="2" t="s">
+      <c r="L68" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M68" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>113</v>
       </c>
@@ -3364,10 +3610,10 @@
         <v>7</v>
       </c>
       <c r="F69" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G69" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H69" t="s">
         <v>16</v>
@@ -3381,11 +3627,14 @@
       <c r="K69" s="2">
         <v>3</v>
       </c>
-      <c r="L69" s="2" t="s">
+      <c r="L69" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M69" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>114</v>
       </c>
@@ -3402,10 +3651,10 @@
         <v>7</v>
       </c>
       <c r="F70" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G70" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H70" t="s">
         <v>16</v>
@@ -3419,11 +3668,14 @@
       <c r="K70" s="2">
         <v>2</v>
       </c>
-      <c r="L70" s="2" t="s">
+      <c r="L70" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M70" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>115</v>
       </c>
@@ -3440,10 +3692,10 @@
         <v>7</v>
       </c>
       <c r="F71" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G71" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H71" t="s">
         <v>16</v>
@@ -3457,21 +3709,25 @@
       <c r="K71" s="2">
         <v>1</v>
       </c>
-      <c r="L71">
+      <c r="L71" s="4">
         <v>126</v>
       </c>
+      <c r="M71" t="s">
+        <v>126</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414C4C5B-E2AC-E34D-B38E-76B4E636C38D}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3480,7 +3736,7 @@
     <col min="10" max="10" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3514,8 +3770,11 @@
       <c r="K1" s="3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3549,8 +3808,11 @@
       <c r="K2" s="3">
         <v>126</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -3584,8 +3846,11 @@
       <c r="K3" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -3619,8 +3884,11 @@
       <c r="K4" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3654,8 +3922,11 @@
       <c r="K5" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -3689,8 +3960,11 @@
       <c r="K6" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -3724,8 +3998,11 @@
       <c r="K7" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -3759,8 +4036,11 @@
       <c r="K8" s="3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -3794,8 +4074,11 @@
       <c r="K9" s="3">
         <v>126</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -3829,8 +4112,11 @@
       <c r="K10" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -3864,8 +4150,11 @@
       <c r="K11" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -3899,8 +4188,11 @@
       <c r="K12" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>85</v>
       </c>
@@ -3934,8 +4226,11 @@
       <c r="K13" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>86</v>
       </c>
@@ -3969,8 +4264,11 @@
       <c r="K14" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -4004,8 +4302,11 @@
       <c r="K15" s="3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>88</v>
       </c>
@@ -4039,8 +4340,11 @@
       <c r="K16" s="3">
         <v>126</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>89</v>
       </c>
@@ -4074,8 +4378,11 @@
       <c r="K17" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>90</v>
       </c>
@@ -4109,8 +4416,11 @@
       <c r="K18" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>91</v>
       </c>
@@ -4144,8 +4454,11 @@
       <c r="K19" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>92</v>
       </c>
@@ -4179,8 +4492,11 @@
       <c r="K20" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -4214,8 +4530,11 @@
       <c r="K21" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -4249,10 +4568,8 @@
       <c r="K22" s="3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J23" t="s">
-        <v>106</v>
+      <c r="L22" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>